<commit_message>
User story-1 test conditions added and User story-2 automation for languages are done
</commit_message>
<xml_diff>
--- a/Project Mars-User Story-1.xlsx
+++ b/Project Mars-User Story-1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ammus\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8975C1F0-B44C-4A45-B047-8287E1DA2560}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DF1F2A-47D8-42CD-BF0A-F2EA60A2EA3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{0D2B5DAA-F4CA-4B43-9F67-0BFE73EB32A2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="156">
   <si>
     <r>
       <t xml:space="preserve">2. As an existing user trying to login with valid credentials </t>
@@ -382,149 +382,6 @@
   </si>
   <si>
     <t>Successful login with valid credentials. Home page is displayed correctly.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Add New</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> button on the language tab.
-2. Enter the language in the empty space you want to add to the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Languages</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">.
-3. Choose one option from the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Choose Language Level.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">4. Click on Add button. </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Skills </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">tab.
-2. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Add New </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">button on the Skills tab.
-3.. Enter the Skill in the empty space you want to add to the Skills.
-4. Choose one option from the Choose Skill Level.
-5. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Add</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> button. </t>
-    </r>
   </si>
   <si>
     <t>User can add a single and upto four languages only to their profile and it is displayed correctly and a popup message is diplayed stating 'Language  has been added' at the right corner of the profile sucessfully.</t>
@@ -1591,99 +1448,13 @@
     <t>Updating a language to the profile</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Click on Languages tab.
-2. Click on pencil icon of the language u want to update.
-3. update the fields which needs to be updated.
-4. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Update </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">button. </t>
-    </r>
-  </si>
-  <si>
     <t>Deleting a language from the profile</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Click on Languages tab.
-2. Click on' </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> ' icon of the language u want to delete.
-</t>
-    </r>
-  </si>
-  <si>
     <t>Updating a Skill to the profile</t>
   </si>
   <si>
     <t>User can add a single or multiple Skill to their profile.</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Click on Skills tab.
-2. Click on pencil icon of the skill you want to update.
-3. update the fields which needs to be updated.
-4. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Update</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> button. </t>
-    </r>
   </si>
   <si>
     <r>
@@ -1919,86 +1690,7 @@
     <t>Update a language with optional parameters</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">1. Click on Languages tab.
-2. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pencil</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> icon of the language u want to update.
-3. update the optional parameter of the language which needs to be updated.
-4. Click on Update button. </t>
-    </r>
-  </si>
-  <si>
     <t>Update a skill with optional parameters</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Click on Skills tab.
-2. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>pencil</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> icon of the Skill you want to update.
-3. update the optional parameter of the language which needs to be updated.
-4. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Update</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> button. </t>
-    </r>
   </si>
   <si>
     <r>
@@ -2147,35 +1839,6 @@
   </si>
   <si>
     <r>
-      <t>1. Click on Languages tab.
-2. Click on</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> pencil icon </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">of the language u want to update.
-3. update the language with duplicate value which you want to be updated.
-4. Click on Update button. </t>
-    </r>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">A popup message is displayed stating </t>
     </r>
     <r>
@@ -2194,12 +1857,6 @@
     <t>Updating a duplicate Skill</t>
   </si>
   <si>
-    <t xml:space="preserve">1. Click on Skill tab.
-2. Click on pencil icon of the skill u want to update.
-3. update the skill with duplicate value which you want to be updated.
-4. Click on Update button. </t>
-  </si>
-  <si>
     <r>
       <t>A popup message is displayed stating that "</t>
     </r>
@@ -2217,56 +1874,6 @@
   </si>
   <si>
     <t>Updating a language with null value</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">1. Click on Languages tab. 
-2. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">pencil icon </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">of the language you want to update with null value.
-3. Give the null value in the language which you want to be updated.
-4. Click on </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Update</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> button. </t>
-    </r>
   </si>
   <si>
     <r>
@@ -2456,6 +2063,437 @@
   </si>
   <si>
     <t>TEST CASE ID-28</t>
+  </si>
+  <si>
+    <t>TEST CONDITIONS</t>
+  </si>
+  <si>
+    <t>Validate Join button on Login page</t>
+  </si>
+  <si>
+    <t>Validate Sign in button on Login page</t>
+  </si>
+  <si>
+    <t>Validate Add New on Language tab</t>
+  </si>
+  <si>
+    <t>Validate Update on Language tab</t>
+  </si>
+  <si>
+    <t>Validate Delete on Language tab</t>
+  </si>
+  <si>
+    <t>Validate Add New on Skills tab</t>
+  </si>
+  <si>
+    <t>Validate Update on Skills tab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate Delete on Skills tab </t>
+  </si>
+  <si>
+    <t>Validate Language tab on Profile Page</t>
+  </si>
+  <si>
+    <t>Validate Skills tab on Profile page</t>
+  </si>
+  <si>
+    <t>Validate Login button on Login page</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Add New</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button on the language tab.
+2. Enter the language in the empty space that needed to be added to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Languages</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+3. Choose one option from the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Choose Language Level.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">4. Click on Add button. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on Languages tab.
+2. Click on pencil icon of the language that needs to be updated.
+3. update the fields which needs to be updated.
+4. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">button. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on Languages tab.
+2. Click on' </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>X</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ' icon of the language needs to be deleted.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Skills </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">tab.
+2. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Add New </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">button on the Skills tab.
+3.. Enter the Skill in the empty space needs to be added to the Skills.
+4. Choose one option from the Choose Skill Level.
+5. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Add</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on Skills tab.
+2. Click on pencil icon of the skill that wanted to be updated.
+3. Edit the fields which needs to be updated.
+4. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Update</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on Languages tab.
+2. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pencil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon of the language that needed to be updated.
+3. update the optional parameter of the language which needs to be updated.
+4. Click on Update button. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on Skills tab.
+2. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>pencil</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> icon of the Skill that needs to be updated.
+3. update the optional parameter of the language which needs to be updated.
+4. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Update</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button. </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>1. Click on Languages tab.
+2. Click on</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> pencil icon </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">of the language that needed to be updated.
+3. update the language with duplicate value which needs to be updated.
+4. Click on Update button. </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Click on Skill tab.
+2. Click on pencil icon of the skill that needs to be updated.
+3. update the skill with duplicate value that needs to be updated.
+4. Click on Update button. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Click on Languages tab. 
+2. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">pencil icon </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">of the language that needs to be updated.
+3. Give the null value in the language which needs to be updated.
+4. Click on </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Update</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> button. </t>
+    </r>
+  </si>
+  <si>
+    <t>Validate language and skills tab on Profile page</t>
   </si>
 </sst>
 </file>
@@ -2590,7 +2628,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -2964,20 +3002,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="136">
+  <cellXfs count="148">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3012,9 +3060,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3033,6 +3078,159 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3041,6 +3239,126 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -3050,86 +3368,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -3140,236 +3380,83 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="180" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3685,1237 +3772,1328 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3A05B08-6E5F-442E-AEA6-3B0C13B4924A}">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:R77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E82" sqref="E82"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71:C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.85546875" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="3" width="51.7109375" customWidth="1"/>
-    <col min="14" max="14" width="7.85546875" customWidth="1"/>
-    <col min="15" max="15" width="3.5703125" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" customWidth="1"/>
+    <col min="4" max="4" width="53.5703125" customWidth="1"/>
+    <col min="15" max="15" width="7.85546875" customWidth="1"/>
+    <col min="16" max="16" width="3.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+    <row r="1" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="94" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-      <c r="J1" s="59"/>
-      <c r="K1" s="59"/>
-      <c r="L1" s="59"/>
-      <c r="M1" s="59"/>
-      <c r="N1" s="59"/>
-      <c r="O1" s="59"/>
-      <c r="P1" s="59"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="B1" s="94"/>
+      <c r="C1" s="94"/>
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="94"/>
+      <c r="O1" s="94"/>
+      <c r="P1" s="94"/>
+      <c r="Q1" s="94"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L2" s="1"/>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L3" s="1"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I4" s="1"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="21" x14ac:dyDescent="0.35">
-      <c r="A18" s="59" t="s">
+    <row r="18" spans="1:18" ht="21" x14ac:dyDescent="0.35">
+      <c r="A18" s="94" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="59"/>
-      <c r="D18" s="59"/>
-      <c r="E18" s="59"/>
-      <c r="F18" s="59"/>
-      <c r="G18" s="59"/>
-      <c r="H18" s="59"/>
-      <c r="I18" s="59"/>
-      <c r="J18" s="59"/>
-      <c r="K18" s="59"/>
-      <c r="L18" s="59"/>
-      <c r="M18" s="59"/>
-      <c r="N18" s="59"/>
-      <c r="O18" s="59"/>
-      <c r="P18" s="59"/>
-      <c r="Q18" s="59"/>
-    </row>
-    <row r="19" spans="1:17" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="B18" s="94"/>
+      <c r="C18" s="94"/>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+      <c r="L18" s="94"/>
+      <c r="M18" s="94"/>
+      <c r="N18" s="94"/>
+      <c r="O18" s="94"/>
+      <c r="P18" s="94"/>
+      <c r="Q18" s="94"/>
+      <c r="R18" s="94"/>
+    </row>
+    <row r="19" spans="1:18" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="17" t="s">
+      <c r="C19" s="53" t="s">
+        <v>133</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="60" t="s">
+      <c r="E19" s="95" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="60"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-      <c r="L19" s="60"/>
-      <c r="M19" s="60"/>
-      <c r="N19" s="60"/>
-      <c r="O19" s="60"/>
-    </row>
-    <row r="20" spans="1:17" ht="105" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="121" t="s">
+      <c r="F19" s="95"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="95"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="95"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+    </row>
+    <row r="20" spans="1:18" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="99" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="72" t="s">
+      <c r="B20" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="126" t="s">
+        <v>134</v>
+      </c>
+      <c r="D20" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="96" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="97"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="97"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="97"/>
+      <c r="M20" s="97"/>
+      <c r="N20" s="97"/>
+      <c r="O20" s="97"/>
+      <c r="P20" s="98"/>
+    </row>
+    <row r="21" spans="1:18" ht="90" x14ac:dyDescent="0.25">
+      <c r="A21" s="100"/>
+      <c r="B21" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" s="127" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="E21" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" s="76"/>
+      <c r="G21" s="76"/>
+      <c r="H21" s="76"/>
+      <c r="I21" s="76"/>
+      <c r="J21" s="76"/>
+      <c r="K21" s="76"/>
+      <c r="L21" s="76"/>
+      <c r="M21" s="76"/>
+      <c r="N21" s="76"/>
+      <c r="O21" s="76"/>
+      <c r="P21" s="108"/>
+    </row>
+    <row r="22" spans="1:18" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="100"/>
+      <c r="B22" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="134" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="E22" s="75" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="76"/>
+      <c r="K22" s="76"/>
+      <c r="L22" s="76"/>
+      <c r="M22" s="76"/>
+      <c r="N22" s="76"/>
+      <c r="O22" s="76"/>
+      <c r="P22" s="108"/>
+    </row>
+    <row r="23" spans="1:18" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="100"/>
+      <c r="B23" s="55"/>
+      <c r="C23" s="135"/>
+      <c r="D23" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="109"/>
+      <c r="F23" s="110"/>
+      <c r="G23" s="110"/>
+      <c r="H23" s="110"/>
+      <c r="I23" s="110"/>
+      <c r="J23" s="110"/>
+      <c r="K23" s="110"/>
+      <c r="L23" s="110"/>
+      <c r="M23" s="110"/>
+      <c r="N23" s="110"/>
+      <c r="O23" s="110"/>
+      <c r="P23" s="111"/>
+    </row>
+    <row r="24" spans="1:18" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="100"/>
+      <c r="B24" s="31" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="136"/>
+      <c r="D24" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="72" t="s">
+        <v>48</v>
+      </c>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73"/>
+      <c r="H24" s="73"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="73"/>
+      <c r="K24" s="73"/>
+      <c r="L24" s="73"/>
+      <c r="M24" s="73"/>
+      <c r="N24" s="73"/>
+      <c r="O24" s="73"/>
+      <c r="P24" s="74"/>
+    </row>
+    <row r="25" spans="1:18" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="100"/>
+      <c r="B25" s="54" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="134" t="s">
+        <v>137</v>
+      </c>
+      <c r="D25" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="88" t="s">
+        <v>83</v>
+      </c>
+      <c r="F25" s="89"/>
+      <c r="G25" s="89"/>
+      <c r="H25" s="89"/>
+      <c r="I25" s="89"/>
+      <c r="J25" s="89"/>
+      <c r="K25" s="89"/>
+      <c r="L25" s="89"/>
+      <c r="M25" s="89"/>
+      <c r="N25" s="89"/>
+      <c r="O25" s="89"/>
+      <c r="P25" s="112"/>
+    </row>
+    <row r="26" spans="1:18" ht="81" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="100"/>
+      <c r="B26" s="55"/>
+      <c r="C26" s="137"/>
+      <c r="D26" s="21" t="s">
+        <v>146</v>
+      </c>
+      <c r="E26" s="91"/>
+      <c r="F26" s="92"/>
+      <c r="G26" s="92"/>
+      <c r="H26" s="92"/>
+      <c r="I26" s="92"/>
+      <c r="J26" s="92"/>
+      <c r="K26" s="92"/>
+      <c r="L26" s="92"/>
+      <c r="M26" s="92"/>
+      <c r="N26" s="92"/>
+      <c r="O26" s="92"/>
+      <c r="P26" s="113"/>
+    </row>
+    <row r="27" spans="1:18" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="100"/>
+      <c r="B27" s="64" t="s">
+        <v>110</v>
+      </c>
+      <c r="C27" s="134" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="37" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="88" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="89"/>
+      <c r="G27" s="89"/>
+      <c r="H27" s="89"/>
+      <c r="I27" s="89"/>
+      <c r="J27" s="89"/>
+      <c r="K27" s="89"/>
+      <c r="L27" s="89"/>
+      <c r="M27" s="89"/>
+      <c r="N27" s="89"/>
+      <c r="O27" s="89"/>
+      <c r="P27" s="112"/>
+    </row>
+    <row r="28" spans="1:18" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="100"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="136"/>
+      <c r="D28" s="34" t="s">
+        <v>147</v>
+      </c>
+      <c r="E28" s="91"/>
+      <c r="F28" s="92"/>
+      <c r="G28" s="92"/>
+      <c r="H28" s="92"/>
+      <c r="I28" s="92"/>
+      <c r="J28" s="92"/>
+      <c r="K28" s="92"/>
+      <c r="L28" s="92"/>
+      <c r="M28" s="92"/>
+      <c r="N28" s="92"/>
+      <c r="O28" s="92"/>
+      <c r="P28" s="113"/>
+    </row>
+    <row r="29" spans="1:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="100"/>
+      <c r="B29" s="54" t="s">
+        <v>111</v>
+      </c>
+      <c r="C29" s="140" t="s">
+        <v>139</v>
+      </c>
+      <c r="D29" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="88" t="s">
+        <v>68</v>
+      </c>
+      <c r="F29" s="89"/>
+      <c r="G29" s="89"/>
+      <c r="H29" s="89"/>
+      <c r="I29" s="89"/>
+      <c r="J29" s="89"/>
+      <c r="K29" s="89"/>
+      <c r="L29" s="89"/>
+      <c r="M29" s="89"/>
+      <c r="N29" s="89"/>
+      <c r="O29" s="89"/>
+      <c r="P29" s="90"/>
+    </row>
+    <row r="30" spans="1:18" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="100"/>
+      <c r="B30" s="55"/>
+      <c r="C30" s="141"/>
+      <c r="D30" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="E30" s="102"/>
+      <c r="F30" s="103"/>
+      <c r="G30" s="103"/>
+      <c r="H30" s="103"/>
+      <c r="I30" s="103"/>
+      <c r="J30" s="103"/>
+      <c r="K30" s="103"/>
+      <c r="L30" s="103"/>
+      <c r="M30" s="103"/>
+      <c r="N30" s="103"/>
+      <c r="O30" s="103"/>
+      <c r="P30" s="104"/>
+    </row>
+    <row r="31" spans="1:18" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="100"/>
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="102"/>
+      <c r="F31" s="103"/>
+      <c r="G31" s="103"/>
+      <c r="H31" s="103"/>
+      <c r="I31" s="103"/>
+      <c r="J31" s="103"/>
+      <c r="K31" s="103"/>
+      <c r="L31" s="103"/>
+      <c r="M31" s="103"/>
+      <c r="N31" s="103"/>
+      <c r="O31" s="103"/>
+      <c r="P31" s="104"/>
+    </row>
+    <row r="32" spans="1:18" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="100"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="51"/>
+      <c r="D32" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="E32" s="85"/>
+      <c r="F32" s="86"/>
+      <c r="G32" s="86"/>
+      <c r="H32" s="86"/>
+      <c r="I32" s="86"/>
+      <c r="J32" s="86"/>
+      <c r="K32" s="86"/>
+      <c r="L32" s="86"/>
+      <c r="M32" s="86"/>
+      <c r="N32" s="86"/>
+      <c r="O32" s="86"/>
+      <c r="P32" s="87"/>
+    </row>
+    <row r="33" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="100"/>
+      <c r="B33" s="64" t="s">
+        <v>112</v>
+      </c>
+      <c r="C33" s="140" t="s">
+        <v>140</v>
+      </c>
+      <c r="D33" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="82" t="s">
+        <v>85</v>
+      </c>
+      <c r="F33" s="83"/>
+      <c r="G33" s="83"/>
+      <c r="H33" s="83"/>
+      <c r="I33" s="83"/>
+      <c r="J33" s="83"/>
+      <c r="K33" s="83"/>
+      <c r="L33" s="83"/>
+      <c r="M33" s="83"/>
+      <c r="N33" s="83"/>
+      <c r="O33" s="83"/>
+      <c r="P33" s="84"/>
+    </row>
+    <row r="34" spans="1:18" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="100"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="130"/>
+      <c r="D34" s="23" t="s">
+        <v>149</v>
+      </c>
+      <c r="E34" s="85"/>
+      <c r="F34" s="86"/>
+      <c r="G34" s="86"/>
+      <c r="H34" s="86"/>
+      <c r="I34" s="86"/>
+      <c r="J34" s="86"/>
+      <c r="K34" s="86"/>
+      <c r="L34" s="86"/>
+      <c r="M34" s="86"/>
+      <c r="N34" s="86"/>
+      <c r="O34" s="86"/>
+      <c r="P34" s="87"/>
+    </row>
+    <row r="35" spans="1:18" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="100"/>
+      <c r="B35" s="66" t="s">
+        <v>113</v>
+      </c>
+      <c r="C35" s="140" t="s">
+        <v>141</v>
+      </c>
+      <c r="D35" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="E35" s="82" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="83"/>
+      <c r="G35" s="83"/>
+      <c r="H35" s="83"/>
+      <c r="I35" s="83"/>
+      <c r="J35" s="83"/>
+      <c r="K35" s="83"/>
+      <c r="L35" s="83"/>
+      <c r="M35" s="83"/>
+      <c r="N35" s="83"/>
+      <c r="O35" s="83"/>
+      <c r="P35" s="84"/>
+    </row>
+    <row r="36" spans="1:18" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="101"/>
+      <c r="B36" s="67"/>
+      <c r="C36" s="142"/>
+      <c r="D36" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="85"/>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="86"/>
+      <c r="I36" s="86"/>
+      <c r="J36" s="86"/>
+      <c r="K36" s="86"/>
+      <c r="L36" s="86"/>
+      <c r="M36" s="86"/>
+      <c r="N36" s="86"/>
+      <c r="O36" s="86"/>
+      <c r="P36" s="87"/>
+    </row>
+    <row r="37" spans="1:18" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="105" t="s">
+        <v>20</v>
+      </c>
+      <c r="B37" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="C37" s="143" t="s">
+        <v>142</v>
+      </c>
+      <c r="D37" s="38" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="82" t="s">
+        <v>59</v>
+      </c>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="83"/>
+      <c r="M37" s="83"/>
+      <c r="N37" s="83"/>
+      <c r="O37" s="83"/>
+      <c r="P37" s="84"/>
+    </row>
+    <row r="38" spans="1:18" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="106"/>
+      <c r="B38" s="55"/>
+      <c r="C38" s="138"/>
+      <c r="D38" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="91"/>
+      <c r="F38" s="92"/>
+      <c r="G38" s="92"/>
+      <c r="H38" s="92"/>
+      <c r="I38" s="92"/>
+      <c r="J38" s="92"/>
+      <c r="K38" s="92"/>
+      <c r="L38" s="92"/>
+      <c r="M38" s="92"/>
+      <c r="N38" s="92"/>
+      <c r="O38" s="92"/>
+      <c r="P38" s="93"/>
+    </row>
+    <row r="39" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="106"/>
+      <c r="B39" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C39" s="138"/>
+      <c r="D39" s="39" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="88" t="s">
+        <v>83</v>
+      </c>
+      <c r="F39" s="89"/>
+      <c r="G39" s="89"/>
+      <c r="H39" s="89"/>
+      <c r="I39" s="89"/>
+      <c r="J39" s="89"/>
+      <c r="K39" s="89"/>
+      <c r="L39" s="89"/>
+      <c r="M39" s="89"/>
+      <c r="N39" s="89"/>
+      <c r="O39" s="89"/>
+      <c r="P39" s="90"/>
+    </row>
+    <row r="40" spans="1:18" ht="93" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="106"/>
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="E40" s="91"/>
+      <c r="F40" s="92"/>
+      <c r="G40" s="92"/>
+      <c r="H40" s="92"/>
+      <c r="I40" s="92"/>
+      <c r="J40" s="92"/>
+      <c r="K40" s="92"/>
+      <c r="L40" s="92"/>
+      <c r="M40" s="92"/>
+      <c r="N40" s="92"/>
+      <c r="O40" s="92"/>
+      <c r="P40" s="93"/>
+    </row>
+    <row r="41" spans="1:18" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="106"/>
+      <c r="B41" s="54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="139" t="s">
+        <v>143</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="88" t="s">
+        <v>57</v>
+      </c>
+      <c r="F41" s="89"/>
+      <c r="G41" s="89"/>
+      <c r="H41" s="89"/>
+      <c r="I41" s="89"/>
+      <c r="J41" s="89"/>
+      <c r="K41" s="89"/>
+      <c r="L41" s="89"/>
+      <c r="M41" s="89"/>
+      <c r="N41" s="89"/>
+      <c r="O41" s="89"/>
+      <c r="P41" s="90"/>
+    </row>
+    <row r="42" spans="1:18" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="106"/>
+      <c r="B42" s="55"/>
+      <c r="C42" s="129"/>
+      <c r="D42" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E42" s="91"/>
+      <c r="F42" s="92"/>
+      <c r="G42" s="92"/>
+      <c r="H42" s="92"/>
+      <c r="I42" s="92"/>
+      <c r="J42" s="92"/>
+      <c r="K42" s="92"/>
+      <c r="L42" s="92"/>
+      <c r="M42" s="92"/>
+      <c r="N42" s="92"/>
+      <c r="O42" s="92"/>
+      <c r="P42" s="93"/>
+    </row>
+    <row r="43" spans="1:18" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="106"/>
+      <c r="B43" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="C43" s="129"/>
+      <c r="D43" s="41" t="s">
+        <v>92</v>
+      </c>
+      <c r="E43" s="88" t="s">
+        <v>93</v>
+      </c>
+      <c r="F43" s="89"/>
+      <c r="G43" s="89"/>
+      <c r="H43" s="89"/>
+      <c r="I43" s="89"/>
+      <c r="J43" s="89"/>
+      <c r="K43" s="89"/>
+      <c r="L43" s="89"/>
+      <c r="M43" s="89"/>
+      <c r="N43" s="89"/>
+      <c r="O43" s="89"/>
+      <c r="P43" s="112"/>
+    </row>
+    <row r="44" spans="1:18" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="107"/>
+      <c r="B44" s="55"/>
+      <c r="C44" s="128"/>
+      <c r="D44" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="E44" s="91"/>
+      <c r="F44" s="92"/>
+      <c r="G44" s="92"/>
+      <c r="H44" s="92"/>
+      <c r="I44" s="92"/>
+      <c r="J44" s="92"/>
+      <c r="K44" s="92"/>
+      <c r="L44" s="92"/>
+      <c r="M44" s="92"/>
+      <c r="N44" s="92"/>
+      <c r="O44" s="92"/>
+      <c r="P44" s="113"/>
+    </row>
+    <row r="45" spans="1:18" s="9" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C45" s="144" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="D20" s="61" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
-      <c r="L20" s="62"/>
-      <c r="M20" s="62"/>
-      <c r="N20" s="62"/>
-      <c r="O20" s="63"/>
-    </row>
-    <row r="21" spans="1:17" ht="90" x14ac:dyDescent="0.25">
-      <c r="A21" s="122"/>
-      <c r="B21" s="87" t="s">
-        <v>116</v>
-      </c>
-      <c r="C21" s="7" t="s">
+      <c r="E45" s="72" t="s">
+        <v>58</v>
+      </c>
+      <c r="F45" s="73"/>
+      <c r="G45" s="73"/>
+      <c r="H45" s="73"/>
+      <c r="I45" s="73"/>
+      <c r="J45" s="73"/>
+      <c r="K45" s="73"/>
+      <c r="L45" s="73"/>
+      <c r="M45" s="73"/>
+      <c r="N45" s="73"/>
+      <c r="O45" s="73"/>
+      <c r="P45" s="118"/>
+      <c r="Q45" s="10"/>
+      <c r="R45" s="10"/>
+    </row>
+    <row r="46" spans="1:18" s="9" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="59"/>
+      <c r="B46" s="26" t="s">
+        <v>119</v>
+      </c>
+      <c r="C46" s="145" t="s">
+        <v>144</v>
+      </c>
+      <c r="D46" s="13" t="s">
         <v>95</v>
       </c>
-      <c r="D21" s="40" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="41"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="41"/>
-      <c r="L21" s="41"/>
-      <c r="M21" s="41"/>
-      <c r="N21" s="41"/>
-      <c r="O21" s="42"/>
-    </row>
-    <row r="22" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="122"/>
-      <c r="B22" s="97" t="s">
-        <v>117</v>
-      </c>
-      <c r="C22" s="106" t="s">
-        <v>22</v>
-      </c>
-      <c r="D22" s="29" t="s">
+      <c r="E46" s="72" t="s">
+        <v>51</v>
+      </c>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
+      <c r="I46" s="73"/>
+      <c r="J46" s="73"/>
+      <c r="K46" s="73"/>
+      <c r="L46" s="73"/>
+      <c r="M46" s="73"/>
+      <c r="N46" s="73"/>
+      <c r="O46" s="73"/>
+      <c r="P46" s="118"/>
+      <c r="Q46" s="11"/>
+    </row>
+    <row r="47" spans="1:18" s="9" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="59"/>
+      <c r="B47" s="54" t="s">
+        <v>120</v>
+      </c>
+      <c r="C47" s="139" t="s">
+        <v>142</v>
+      </c>
+      <c r="D47" s="42" t="s">
+        <v>27</v>
+      </c>
+      <c r="E47" s="75" t="s">
+        <v>71</v>
+      </c>
+      <c r="F47" s="76"/>
+      <c r="G47" s="76"/>
+      <c r="H47" s="76"/>
+      <c r="I47" s="76"/>
+      <c r="J47" s="76"/>
+      <c r="K47" s="76"/>
+      <c r="L47" s="76"/>
+      <c r="M47" s="76"/>
+      <c r="N47" s="76"/>
+      <c r="O47" s="76"/>
+      <c r="P47" s="108"/>
+      <c r="Q47" s="11"/>
+    </row>
+    <row r="48" spans="1:18" s="9" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" s="59"/>
+      <c r="B48" s="55"/>
+      <c r="C48" s="129"/>
+      <c r="D48" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E48" s="78"/>
+      <c r="F48" s="79"/>
+      <c r="G48" s="79"/>
+      <c r="H48" s="79"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="79"/>
+      <c r="L48" s="79"/>
+      <c r="M48" s="79"/>
+      <c r="N48" s="79"/>
+      <c r="O48" s="79"/>
+      <c r="P48" s="114"/>
+      <c r="Q48" s="11"/>
+    </row>
+    <row r="49" spans="1:17" s="9" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="59"/>
+      <c r="B49" s="33"/>
+      <c r="C49" s="129"/>
+      <c r="D49" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="E49" s="69" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="70"/>
+      <c r="G49" s="70"/>
+      <c r="H49" s="70"/>
+      <c r="I49" s="70"/>
+      <c r="J49" s="70"/>
+      <c r="K49" s="70"/>
+      <c r="L49" s="70"/>
+      <c r="M49" s="70"/>
+      <c r="N49" s="70"/>
+      <c r="O49" s="70"/>
+      <c r="P49" s="71"/>
+      <c r="Q49" s="11"/>
+    </row>
+    <row r="50" spans="1:17" s="9" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="59"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="129"/>
+      <c r="D50" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="119" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="120"/>
+      <c r="G50" s="120"/>
+      <c r="H50" s="120"/>
+      <c r="I50" s="120"/>
+      <c r="J50" s="120"/>
+      <c r="K50" s="120"/>
+      <c r="L50" s="120"/>
+      <c r="M50" s="120"/>
+      <c r="N50" s="120"/>
+      <c r="O50" s="120"/>
+      <c r="P50" s="121"/>
+      <c r="Q50" s="11"/>
+    </row>
+    <row r="51" spans="1:17" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="59"/>
+      <c r="B51" s="54" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="129"/>
+      <c r="D51" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="E51" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="F51" s="76"/>
+      <c r="G51" s="76"/>
+      <c r="H51" s="76"/>
+      <c r="I51" s="76"/>
+      <c r="J51" s="76"/>
+      <c r="K51" s="76"/>
+      <c r="L51" s="76"/>
+      <c r="M51" s="76"/>
+      <c r="N51" s="76"/>
+      <c r="O51" s="76"/>
+      <c r="P51" s="108"/>
+    </row>
+    <row r="52" spans="1:17" s="10" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="59"/>
+      <c r="B52" s="55"/>
+      <c r="C52" s="128"/>
+      <c r="D52" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="E52" s="78"/>
+      <c r="F52" s="79"/>
+      <c r="G52" s="79"/>
+      <c r="H52" s="79"/>
+      <c r="I52" s="79"/>
+      <c r="J52" s="79"/>
+      <c r="K52" s="79"/>
+      <c r="L52" s="79"/>
+      <c r="M52" s="79"/>
+      <c r="N52" s="79"/>
+      <c r="O52" s="79"/>
+      <c r="P52" s="114"/>
+    </row>
+    <row r="53" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="59"/>
+      <c r="B53" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="C53" s="139" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E53" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="F53" s="76"/>
+      <c r="G53" s="76"/>
+      <c r="H53" s="76"/>
+      <c r="I53" s="76"/>
+      <c r="J53" s="76"/>
+      <c r="K53" s="76"/>
+      <c r="L53" s="76"/>
+      <c r="M53" s="76"/>
+      <c r="N53" s="76"/>
+      <c r="O53" s="76"/>
+      <c r="P53" s="108"/>
+    </row>
+    <row r="54" spans="1:17" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="59"/>
+      <c r="B54" s="55"/>
+      <c r="C54" s="129"/>
+      <c r="D54" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E54" s="78"/>
+      <c r="F54" s="79"/>
+      <c r="G54" s="79"/>
+      <c r="H54" s="79"/>
+      <c r="I54" s="79"/>
+      <c r="J54" s="79"/>
+      <c r="K54" s="79"/>
+      <c r="L54" s="79"/>
+      <c r="M54" s="79"/>
+      <c r="N54" s="79"/>
+      <c r="O54" s="79"/>
+      <c r="P54" s="114"/>
+    </row>
+    <row r="55" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="59"/>
+      <c r="B55" s="33"/>
+      <c r="C55" s="129"/>
+      <c r="D55" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="E55" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="F55" s="70"/>
+      <c r="G55" s="70"/>
+      <c r="H55" s="70"/>
+      <c r="I55" s="70"/>
+      <c r="J55" s="70"/>
+      <c r="K55" s="70"/>
+      <c r="L55" s="70"/>
+      <c r="M55" s="70"/>
+      <c r="N55" s="70"/>
+      <c r="O55" s="70"/>
+      <c r="P55" s="71"/>
+    </row>
+    <row r="56" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="59"/>
+      <c r="B56" s="33"/>
+      <c r="C56" s="129"/>
+      <c r="D56" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E56" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="F56" s="70"/>
+      <c r="G56" s="70"/>
+      <c r="H56" s="70"/>
+      <c r="I56" s="70"/>
+      <c r="J56" s="70"/>
+      <c r="K56" s="70"/>
+      <c r="L56" s="70"/>
+      <c r="M56" s="70"/>
+      <c r="N56" s="70"/>
+      <c r="O56" s="70"/>
+      <c r="P56" s="71"/>
+    </row>
+    <row r="57" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="59"/>
+      <c r="B57" s="54" t="s">
+        <v>123</v>
+      </c>
+      <c r="C57" s="129"/>
+      <c r="D57" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="E57" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="F57" s="76"/>
+      <c r="G57" s="76"/>
+      <c r="H57" s="76"/>
+      <c r="I57" s="76"/>
+      <c r="J57" s="76"/>
+      <c r="K57" s="76"/>
+      <c r="L57" s="76"/>
+      <c r="M57" s="76"/>
+      <c r="N57" s="76"/>
+      <c r="O57" s="76"/>
+      <c r="P57" s="77"/>
+    </row>
+    <row r="58" spans="1:17" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="60"/>
+      <c r="B58" s="55"/>
+      <c r="C58" s="128"/>
+      <c r="D58" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="E58" s="78"/>
+      <c r="F58" s="79"/>
+      <c r="G58" s="79"/>
+      <c r="H58" s="79"/>
+      <c r="I58" s="79"/>
+      <c r="J58" s="79"/>
+      <c r="K58" s="79"/>
+      <c r="L58" s="79"/>
+      <c r="M58" s="79"/>
+      <c r="N58" s="79"/>
+      <c r="O58" s="79"/>
+      <c r="P58" s="80"/>
+    </row>
+    <row r="59" spans="1:17" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="B59" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C59" s="146" t="s">
+        <v>134</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="E59" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="F59" s="73"/>
+      <c r="G59" s="73"/>
+      <c r="H59" s="73"/>
+      <c r="I59" s="73"/>
+      <c r="J59" s="73"/>
+      <c r="K59" s="73"/>
+      <c r="L59" s="73"/>
+      <c r="M59" s="73"/>
+      <c r="N59" s="73"/>
+      <c r="O59" s="73"/>
+      <c r="P59" s="74"/>
+    </row>
+    <row r="60" spans="1:17" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="62"/>
+      <c r="B60" s="26" t="s">
+        <v>125</v>
+      </c>
+      <c r="C60" s="146" t="s">
+        <v>144</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="E60" s="72" t="s">
+        <v>64</v>
+      </c>
+      <c r="F60" s="73"/>
+      <c r="G60" s="73"/>
+      <c r="H60" s="73"/>
+      <c r="I60" s="73"/>
+      <c r="J60" s="73"/>
+      <c r="K60" s="73"/>
+      <c r="L60" s="73"/>
+      <c r="M60" s="73"/>
+      <c r="N60" s="73"/>
+      <c r="O60" s="73"/>
+      <c r="P60" s="74"/>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A61" s="62"/>
+      <c r="B61" s="54" t="s">
+        <v>126</v>
+      </c>
+      <c r="C61" s="131" t="s">
+        <v>142</v>
+      </c>
+      <c r="D61" s="40" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="75" t="s">
+        <v>73</v>
+      </c>
+      <c r="F61" s="76"/>
+      <c r="G61" s="76"/>
+      <c r="H61" s="76"/>
+      <c r="I61" s="76"/>
+      <c r="J61" s="76"/>
+      <c r="K61" s="76"/>
+      <c r="L61" s="76"/>
+      <c r="M61" s="76"/>
+      <c r="N61" s="76"/>
+      <c r="O61" s="76"/>
+      <c r="P61" s="77"/>
+    </row>
+    <row r="62" spans="1:17" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="62"/>
+      <c r="B62" s="55"/>
+      <c r="C62" s="132"/>
+      <c r="D62" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="E62" s="78"/>
+      <c r="F62" s="79"/>
+      <c r="G62" s="79"/>
+      <c r="H62" s="79"/>
+      <c r="I62" s="79"/>
+      <c r="J62" s="79"/>
+      <c r="K62" s="79"/>
+      <c r="L62" s="79"/>
+      <c r="M62" s="79"/>
+      <c r="N62" s="79"/>
+      <c r="O62" s="79"/>
+      <c r="P62" s="80"/>
+    </row>
+    <row r="63" spans="1:17" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="62"/>
+      <c r="B63" s="26" t="s">
+        <v>127</v>
+      </c>
+      <c r="C63" s="132"/>
+      <c r="D63" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E63" s="69" t="s">
+        <v>74</v>
+      </c>
+      <c r="F63" s="70"/>
+      <c r="G63" s="70"/>
+      <c r="H63" s="70"/>
+      <c r="I63" s="70"/>
+      <c r="J63" s="70"/>
+      <c r="K63" s="70"/>
+      <c r="L63" s="70"/>
+      <c r="M63" s="70"/>
+      <c r="N63" s="70"/>
+      <c r="O63" s="70"/>
+      <c r="P63" s="81"/>
+    </row>
+    <row r="64" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="62"/>
+      <c r="B64" s="54" t="s">
+        <v>128</v>
+      </c>
+      <c r="C64" s="132"/>
+      <c r="D64" s="46" t="s">
+        <v>100</v>
+      </c>
+      <c r="E64" s="75" t="s">
+        <v>101</v>
+      </c>
+      <c r="F64" s="76"/>
+      <c r="G64" s="76"/>
+      <c r="H64" s="76"/>
+      <c r="I64" s="76"/>
+      <c r="J64" s="76"/>
+      <c r="K64" s="76"/>
+      <c r="L64" s="76"/>
+      <c r="M64" s="76"/>
+      <c r="N64" s="76"/>
+      <c r="O64" s="76"/>
+      <c r="P64" s="77"/>
+    </row>
+    <row r="65" spans="1:16" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="62"/>
+      <c r="B65" s="55"/>
+      <c r="C65" s="133"/>
+      <c r="D65" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="E65" s="78"/>
+      <c r="F65" s="79"/>
+      <c r="G65" s="79"/>
+      <c r="H65" s="79"/>
+      <c r="I65" s="79"/>
+      <c r="J65" s="79"/>
+      <c r="K65" s="79"/>
+      <c r="L65" s="79"/>
+      <c r="M65" s="79"/>
+      <c r="N65" s="79"/>
+      <c r="O65" s="79"/>
+      <c r="P65" s="80"/>
+    </row>
+    <row r="66" spans="1:16" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="62"/>
+      <c r="B66" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="C66" s="139" t="s">
+        <v>143</v>
+      </c>
+      <c r="D66" s="47" t="s">
+        <v>35</v>
+      </c>
+      <c r="E66" s="75" t="s">
+        <v>75</v>
+      </c>
+      <c r="F66" s="76"/>
+      <c r="G66" s="76"/>
+      <c r="H66" s="76"/>
+      <c r="I66" s="76"/>
+      <c r="J66" s="76"/>
+      <c r="K66" s="76"/>
+      <c r="L66" s="76"/>
+      <c r="M66" s="76"/>
+      <c r="N66" s="76"/>
+      <c r="O66" s="76"/>
+      <c r="P66" s="77"/>
+    </row>
+    <row r="67" spans="1:16" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="62"/>
+      <c r="B67" s="55"/>
+      <c r="C67" s="129"/>
+      <c r="D67" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="E22" s="30"/>
-      <c r="F22" s="30"/>
-      <c r="G22" s="30"/>
-      <c r="H22" s="30"/>
-      <c r="I22" s="30"/>
-      <c r="J22" s="30"/>
-      <c r="K22" s="30"/>
-      <c r="L22" s="30"/>
-      <c r="M22" s="30"/>
-      <c r="N22" s="30"/>
-      <c r="O22" s="39"/>
-    </row>
-    <row r="23" spans="1:17" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="122"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="83"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="84"/>
-      <c r="M23" s="84"/>
-      <c r="N23" s="84"/>
-      <c r="O23" s="85"/>
-    </row>
-    <row r="24" spans="1:17" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="122"/>
-      <c r="B24" s="87" t="s">
-        <v>118</v>
-      </c>
-      <c r="C24" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>50</v>
-      </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="24"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="24"/>
-      <c r="N24" s="24"/>
-      <c r="O24" s="25"/>
-    </row>
-    <row r="25" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="122"/>
-      <c r="B25" s="97" t="s">
-        <v>119</v>
-      </c>
-      <c r="C25" s="107" t="s">
-        <v>81</v>
-      </c>
-      <c r="D25" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
-      <c r="G25" s="41"/>
-      <c r="H25" s="41"/>
-      <c r="I25" s="41"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="67"/>
-    </row>
-    <row r="26" spans="1:17" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="122"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="52"/>
-      <c r="E26" s="53"/>
-      <c r="F26" s="53"/>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="53"/>
-      <c r="L26" s="53"/>
-      <c r="M26" s="53"/>
-      <c r="N26" s="53"/>
-      <c r="O26" s="68"/>
-    </row>
-    <row r="27" spans="1:17" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="122"/>
-      <c r="B27" s="98" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="107" t="s">
-        <v>83</v>
-      </c>
-      <c r="D27" s="40" t="s">
-        <v>89</v>
-      </c>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
-      <c r="G27" s="41"/>
-      <c r="H27" s="41"/>
-      <c r="I27" s="41"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="41"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="41"/>
-      <c r="N27" s="41"/>
-      <c r="O27" s="67"/>
-    </row>
-    <row r="28" spans="1:17" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="122"/>
-      <c r="B28" s="99"/>
-      <c r="C28" s="93" t="s">
-        <v>84</v>
-      </c>
-      <c r="D28" s="52"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="53"/>
-      <c r="K28" s="53"/>
-      <c r="L28" s="53"/>
-      <c r="M28" s="53"/>
-      <c r="N28" s="53"/>
-      <c r="O28" s="68"/>
-    </row>
-    <row r="29" spans="1:17" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="122"/>
-      <c r="B29" s="95" t="s">
-        <v>121</v>
-      </c>
-      <c r="C29" s="71" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="40" t="s">
+      <c r="E67" s="78"/>
+      <c r="F67" s="79"/>
+      <c r="G67" s="79"/>
+      <c r="H67" s="79"/>
+      <c r="I67" s="79"/>
+      <c r="J67" s="79"/>
+      <c r="K67" s="79"/>
+      <c r="L67" s="79"/>
+      <c r="M67" s="79"/>
+      <c r="N67" s="79"/>
+      <c r="O67" s="79"/>
+      <c r="P67" s="80"/>
+    </row>
+    <row r="68" spans="1:16" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="62"/>
+      <c r="B68" s="32" t="s">
+        <v>130</v>
+      </c>
+      <c r="C68" s="129"/>
+      <c r="D68" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
-      <c r="G29" s="41"/>
-      <c r="H29" s="41"/>
-      <c r="I29" s="41"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="41"/>
-      <c r="L29" s="41"/>
-      <c r="M29" s="41"/>
-      <c r="N29" s="41"/>
-      <c r="O29" s="42"/>
-    </row>
-    <row r="30" spans="1:17" ht="88.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="122"/>
-      <c r="B30" s="94"/>
-      <c r="C30" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="43"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
-      <c r="K30" s="44"/>
-      <c r="L30" s="44"/>
-      <c r="M30" s="44"/>
-      <c r="N30" s="44"/>
-      <c r="O30" s="45"/>
-    </row>
-    <row r="31" spans="1:17" ht="24.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="122"/>
-      <c r="B31" s="86"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="44"/>
-      <c r="F31" s="44"/>
-      <c r="G31" s="44"/>
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
-      <c r="K31" s="44"/>
-      <c r="L31" s="44"/>
-      <c r="M31" s="44"/>
-      <c r="N31" s="44"/>
-      <c r="O31" s="45"/>
-    </row>
-    <row r="32" spans="1:17" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="122"/>
-      <c r="B32" s="7"/>
-      <c r="C32" s="70" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="46"/>
-      <c r="E32" s="47"/>
-      <c r="F32" s="47"/>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47"/>
-      <c r="I32" s="47"/>
-      <c r="J32" s="47"/>
-      <c r="K32" s="47"/>
-      <c r="L32" s="47"/>
-      <c r="M32" s="47"/>
-      <c r="N32" s="47"/>
-      <c r="O32" s="48"/>
-    </row>
-    <row r="33" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="122"/>
-      <c r="B33" s="98" t="s">
-        <v>122</v>
-      </c>
-      <c r="C33" s="82" t="s">
-        <v>85</v>
-      </c>
-      <c r="D33" s="49" t="s">
-        <v>90</v>
-      </c>
-      <c r="E33" s="50"/>
-      <c r="F33" s="50"/>
-      <c r="G33" s="50"/>
-      <c r="H33" s="50"/>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50"/>
-      <c r="K33" s="50"/>
-      <c r="L33" s="50"/>
-      <c r="M33" s="50"/>
-      <c r="N33" s="50"/>
-      <c r="O33" s="51"/>
-    </row>
-    <row r="34" spans="1:17" ht="63" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="122"/>
-      <c r="B34" s="99"/>
-      <c r="C34" s="69" t="s">
-        <v>87</v>
-      </c>
-      <c r="D34" s="46"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="47"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="47"/>
-      <c r="I34" s="47"/>
-      <c r="J34" s="47"/>
-      <c r="K34" s="47"/>
-      <c r="L34" s="47"/>
-      <c r="M34" s="47"/>
-      <c r="N34" s="47"/>
-      <c r="O34" s="48"/>
-    </row>
-    <row r="35" spans="1:17" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="122"/>
-      <c r="B35" s="100" t="s">
-        <v>123</v>
-      </c>
-      <c r="C35" s="71" t="s">
-        <v>91</v>
-      </c>
-      <c r="D35" s="49" t="s">
-        <v>93</v>
-      </c>
-      <c r="E35" s="50"/>
-      <c r="F35" s="50"/>
-      <c r="G35" s="50"/>
-      <c r="H35" s="50"/>
-      <c r="I35" s="50"/>
-      <c r="J35" s="50"/>
-      <c r="K35" s="50"/>
-      <c r="L35" s="50"/>
-      <c r="M35" s="50"/>
-      <c r="N35" s="50"/>
-      <c r="O35" s="51"/>
-    </row>
-    <row r="36" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="123"/>
-      <c r="B36" s="101"/>
-      <c r="C36" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="D36" s="46"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
-      <c r="O36" s="48"/>
-    </row>
-    <row r="37" spans="1:17" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="124" t="s">
-        <v>20</v>
-      </c>
-      <c r="B37" s="102" t="s">
-        <v>124</v>
-      </c>
-      <c r="C37" s="108" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="49" t="s">
-        <v>61</v>
-      </c>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="50"/>
-      <c r="O37" s="51"/>
-    </row>
-    <row r="38" spans="1:17" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="125"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D38" s="52"/>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="53"/>
-      <c r="L38" s="53"/>
-      <c r="M38" s="53"/>
-      <c r="N38" s="53"/>
-      <c r="O38" s="54"/>
-    </row>
-    <row r="39" spans="1:17" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="125"/>
-      <c r="B39" s="97" t="s">
-        <v>125</v>
-      </c>
-      <c r="C39" s="109" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="40" t="s">
-        <v>88</v>
-      </c>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="41"/>
-      <c r="L39" s="41"/>
-      <c r="M39" s="41"/>
-      <c r="N39" s="41"/>
-      <c r="O39" s="42"/>
-    </row>
-    <row r="40" spans="1:17" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="125"/>
-      <c r="B40" s="96"/>
-      <c r="C40" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="52"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="53"/>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="53"/>
-      <c r="K40" s="53"/>
-      <c r="L40" s="53"/>
-      <c r="M40" s="53"/>
-      <c r="N40" s="53"/>
-      <c r="O40" s="54"/>
-    </row>
-    <row r="41" spans="1:17" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="125"/>
-      <c r="B41" s="97" t="s">
-        <v>126</v>
-      </c>
-      <c r="C41" s="110" t="s">
-        <v>25</v>
-      </c>
-      <c r="D41" s="40" t="s">
-        <v>59</v>
-      </c>
-      <c r="E41" s="41"/>
-      <c r="F41" s="41"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="41"/>
-      <c r="I41" s="41"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="41"/>
-      <c r="M41" s="41"/>
-      <c r="N41" s="41"/>
-      <c r="O41" s="42"/>
-    </row>
-    <row r="42" spans="1:17" ht="93.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="125"/>
-      <c r="B42" s="96"/>
-      <c r="C42" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="D42" s="52"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="53"/>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="53"/>
-      <c r="L42" s="53"/>
-      <c r="M42" s="53"/>
-      <c r="N42" s="53"/>
-      <c r="O42" s="54"/>
-    </row>
-    <row r="43" spans="1:17" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="125"/>
-      <c r="B43" s="97" t="s">
-        <v>127</v>
-      </c>
-      <c r="C43" s="111" t="s">
-        <v>98</v>
-      </c>
-      <c r="D43" s="40" t="s">
-        <v>100</v>
-      </c>
-      <c r="E43" s="41"/>
-      <c r="F43" s="41"/>
-      <c r="G43" s="41"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="41"/>
-      <c r="L43" s="41"/>
-      <c r="M43" s="41"/>
-      <c r="N43" s="41"/>
-      <c r="O43" s="67"/>
-    </row>
-    <row r="44" spans="1:17" ht="82.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="126"/>
-      <c r="B44" s="96"/>
-      <c r="C44" s="66" t="s">
-        <v>99</v>
-      </c>
-      <c r="D44" s="52"/>
-      <c r="E44" s="53"/>
-      <c r="F44" s="53"/>
-      <c r="G44" s="53"/>
-      <c r="H44" s="53"/>
-      <c r="I44" s="53"/>
-      <c r="J44" s="53"/>
-      <c r="K44" s="53"/>
-      <c r="L44" s="53"/>
-      <c r="M44" s="53"/>
-      <c r="N44" s="53"/>
-      <c r="O44" s="68"/>
-    </row>
-    <row r="45" spans="1:17" s="10" customFormat="1" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="127" t="s">
-        <v>26</v>
-      </c>
-      <c r="B45" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" s="73" t="s">
-        <v>101</v>
-      </c>
-      <c r="D45" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-      <c r="L45" s="24"/>
-      <c r="M45" s="24"/>
-      <c r="N45" s="24"/>
-      <c r="O45" s="65"/>
-      <c r="P45" s="11"/>
-      <c r="Q45" s="11"/>
-    </row>
-    <row r="46" spans="1:17" s="10" customFormat="1" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="128"/>
-      <c r="B46" s="72" t="s">
-        <v>129</v>
-      </c>
-      <c r="C46" s="14" t="s">
+      <c r="E68" s="69" t="s">
+        <v>76</v>
+      </c>
+      <c r="F68" s="70"/>
+      <c r="G68" s="70"/>
+      <c r="H68" s="70"/>
+      <c r="I68" s="70"/>
+      <c r="J68" s="70"/>
+      <c r="K68" s="70"/>
+      <c r="L68" s="70"/>
+      <c r="M68" s="70"/>
+      <c r="N68" s="70"/>
+      <c r="O68" s="70"/>
+      <c r="P68" s="81"/>
+    </row>
+    <row r="69" spans="1:16" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="62"/>
+      <c r="B69" s="54" t="s">
+        <v>131</v>
+      </c>
+      <c r="C69" s="129"/>
+      <c r="D69" s="48" t="s">
         <v>102</v>
       </c>
-      <c r="D46" s="23" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46" s="24"/>
-      <c r="F46" s="24"/>
-      <c r="G46" s="24"/>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24"/>
-      <c r="J46" s="24"/>
-      <c r="K46" s="24"/>
-      <c r="L46" s="24"/>
-      <c r="M46" s="24"/>
-      <c r="N46" s="24"/>
-      <c r="O46" s="65"/>
-      <c r="P46" s="12"/>
-    </row>
-    <row r="47" spans="1:17" s="10" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="128"/>
-      <c r="B47" s="97" t="s">
-        <v>130</v>
-      </c>
-      <c r="C47" s="112" t="s">
-        <v>27</v>
-      </c>
-      <c r="D47" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="E47" s="30"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="30"/>
-      <c r="H47" s="30"/>
-      <c r="I47" s="30"/>
-      <c r="J47" s="30"/>
-      <c r="K47" s="30"/>
-      <c r="L47" s="30"/>
-      <c r="M47" s="30"/>
-      <c r="N47" s="30"/>
-      <c r="O47" s="39"/>
-      <c r="P47" s="12"/>
-    </row>
-    <row r="48" spans="1:17" s="10" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A48" s="128"/>
-      <c r="B48" s="96"/>
-      <c r="C48" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D48" s="32"/>
-      <c r="E48" s="33"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="33"/>
-      <c r="H48" s="33"/>
-      <c r="I48" s="33"/>
-      <c r="J48" s="33"/>
-      <c r="K48" s="33"/>
-      <c r="L48" s="33"/>
-      <c r="M48" s="33"/>
-      <c r="N48" s="33"/>
-      <c r="O48" s="55"/>
-      <c r="P48" s="12"/>
-    </row>
-    <row r="49" spans="1:16" s="10" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="128"/>
-      <c r="B49" s="89"/>
-      <c r="C49" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D49" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="E49" s="36"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="36"/>
-      <c r="H49" s="36"/>
-      <c r="I49" s="36"/>
-      <c r="J49" s="36"/>
-      <c r="K49" s="36"/>
-      <c r="L49" s="36"/>
-      <c r="M49" s="36"/>
-      <c r="N49" s="36"/>
-      <c r="O49" s="38"/>
-      <c r="P49" s="12"/>
-    </row>
-    <row r="50" spans="1:16" s="10" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="128"/>
-      <c r="B50" s="89"/>
-      <c r="C50" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D50" s="56" t="s">
-        <v>29</v>
-      </c>
-      <c r="E50" s="57"/>
-      <c r="F50" s="57"/>
-      <c r="G50" s="57"/>
-      <c r="H50" s="57"/>
-      <c r="I50" s="57"/>
-      <c r="J50" s="57"/>
-      <c r="K50" s="57"/>
-      <c r="L50" s="57"/>
-      <c r="M50" s="57"/>
-      <c r="N50" s="57"/>
-      <c r="O50" s="58"/>
-      <c r="P50" s="12"/>
-    </row>
-    <row r="51" spans="1:16" s="74" customFormat="1" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="128"/>
-      <c r="B51" s="97" t="s">
-        <v>131</v>
-      </c>
-      <c r="C51" s="113" t="s">
-        <v>103</v>
-      </c>
-      <c r="D51" s="29" t="s">
-        <v>105</v>
-      </c>
-      <c r="E51" s="30"/>
-      <c r="F51" s="30"/>
-      <c r="G51" s="30"/>
-      <c r="H51" s="30"/>
-      <c r="I51" s="30"/>
-      <c r="J51" s="30"/>
-      <c r="K51" s="30"/>
-      <c r="L51" s="30"/>
-      <c r="M51" s="30"/>
-      <c r="N51" s="30"/>
-      <c r="O51" s="39"/>
-    </row>
-    <row r="52" spans="1:16" s="74" customFormat="1" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="128"/>
-      <c r="B52" s="96"/>
-      <c r="C52" s="14" t="s">
+      <c r="E69" s="75" t="s">
         <v>104</v>
       </c>
-      <c r="D52" s="32"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="33"/>
-      <c r="G52" s="33"/>
-      <c r="H52" s="33"/>
-      <c r="I52" s="33"/>
-      <c r="J52" s="33"/>
-      <c r="K52" s="33"/>
-      <c r="L52" s="33"/>
-      <c r="M52" s="33"/>
-      <c r="N52" s="33"/>
-      <c r="O52" s="55"/>
-    </row>
-    <row r="53" spans="1:16" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="128"/>
-      <c r="B53" s="97" t="s">
-        <v>132</v>
-      </c>
-      <c r="C53" s="114" t="s">
-        <v>30</v>
-      </c>
-      <c r="D53" s="29" t="s">
-        <v>74</v>
-      </c>
-      <c r="E53" s="30"/>
-      <c r="F53" s="30"/>
-      <c r="G53" s="30"/>
-      <c r="H53" s="30"/>
-      <c r="I53" s="30"/>
-      <c r="J53" s="30"/>
-      <c r="K53" s="30"/>
-      <c r="L53" s="30"/>
-      <c r="M53" s="30"/>
-      <c r="N53" s="30"/>
-      <c r="O53" s="39"/>
-    </row>
-    <row r="54" spans="1:16" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="128"/>
-      <c r="B54" s="96"/>
-      <c r="C54" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D54" s="32"/>
-      <c r="E54" s="33"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="33"/>
-      <c r="H54" s="33"/>
-      <c r="I54" s="33"/>
-      <c r="J54" s="33"/>
-      <c r="K54" s="33"/>
-      <c r="L54" s="33"/>
-      <c r="M54" s="33"/>
-      <c r="N54" s="33"/>
-      <c r="O54" s="55"/>
-    </row>
-    <row r="55" spans="1:16" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="128"/>
-      <c r="B55" s="89"/>
-      <c r="C55" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="35" t="s">
-        <v>57</v>
-      </c>
-      <c r="E55" s="36"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="36"/>
-      <c r="H55" s="36"/>
-      <c r="I55" s="36"/>
-      <c r="J55" s="36"/>
-      <c r="K55" s="36"/>
-      <c r="L55" s="36"/>
-      <c r="M55" s="36"/>
-      <c r="N55" s="36"/>
-      <c r="O55" s="38"/>
-    </row>
-    <row r="56" spans="1:16" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="128"/>
-      <c r="B56" s="89"/>
-      <c r="C56" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="D56" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="E56" s="36"/>
-      <c r="F56" s="36"/>
-      <c r="G56" s="36"/>
-      <c r="H56" s="36"/>
-      <c r="I56" s="36"/>
-      <c r="J56" s="36"/>
-      <c r="K56" s="36"/>
-      <c r="L56" s="36"/>
-      <c r="M56" s="36"/>
-      <c r="N56" s="36"/>
-      <c r="O56" s="38"/>
-    </row>
-    <row r="57" spans="1:16" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="128"/>
-      <c r="B57" s="97" t="s">
-        <v>133</v>
-      </c>
-      <c r="C57" s="115" t="s">
-        <v>106</v>
-      </c>
-      <c r="D57" s="29" t="s">
-        <v>108</v>
-      </c>
-      <c r="E57" s="30"/>
-      <c r="F57" s="30"/>
-      <c r="G57" s="30"/>
-      <c r="H57" s="30"/>
-      <c r="I57" s="30"/>
-      <c r="J57" s="30"/>
-      <c r="K57" s="30"/>
-      <c r="L57" s="30"/>
-      <c r="M57" s="30"/>
-      <c r="N57" s="30"/>
-      <c r="O57" s="31"/>
-    </row>
-    <row r="58" spans="1:16" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="129"/>
-      <c r="B58" s="96"/>
-      <c r="C58" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D58" s="32"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="33"/>
-      <c r="G58" s="33"/>
-      <c r="H58" s="33"/>
-      <c r="I58" s="33"/>
-      <c r="J58" s="33"/>
-      <c r="K58" s="33"/>
-      <c r="L58" s="33"/>
-      <c r="M58" s="33"/>
-      <c r="N58" s="33"/>
-      <c r="O58" s="34"/>
-    </row>
-    <row r="59" spans="1:16" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="130" t="s">
-        <v>33</v>
-      </c>
-      <c r="B59" s="72" t="s">
-        <v>134</v>
-      </c>
-      <c r="C59" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="D59" s="23" t="s">
-        <v>65</v>
-      </c>
-      <c r="E59" s="24"/>
-      <c r="F59" s="24"/>
-      <c r="G59" s="24"/>
-      <c r="H59" s="24"/>
-      <c r="I59" s="24"/>
-      <c r="J59" s="24"/>
-      <c r="K59" s="24"/>
-      <c r="L59" s="24"/>
-      <c r="M59" s="24"/>
-      <c r="N59" s="24"/>
-      <c r="O59" s="25"/>
-    </row>
-    <row r="60" spans="1:16" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="131"/>
-      <c r="B60" s="72" t="s">
-        <v>135</v>
-      </c>
-      <c r="C60" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="D60" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E60" s="24"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="24"/>
-      <c r="H60" s="24"/>
-      <c r="I60" s="24"/>
-      <c r="J60" s="24"/>
-      <c r="K60" s="24"/>
-      <c r="L60" s="24"/>
-      <c r="M60" s="24"/>
-      <c r="N60" s="24"/>
-      <c r="O60" s="25"/>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A61" s="131"/>
-      <c r="B61" s="97" t="s">
-        <v>136</v>
-      </c>
-      <c r="C61" s="110" t="s">
-        <v>34</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>75</v>
-      </c>
-      <c r="E61" s="30"/>
-      <c r="F61" s="30"/>
-      <c r="G61" s="30"/>
-      <c r="H61" s="30"/>
-      <c r="I61" s="30"/>
-      <c r="J61" s="30"/>
-      <c r="K61" s="30"/>
-      <c r="L61" s="30"/>
-      <c r="M61" s="30"/>
-      <c r="N61" s="30"/>
-      <c r="O61" s="31"/>
-    </row>
-    <row r="62" spans="1:16" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="131"/>
-      <c r="B62" s="96"/>
-      <c r="C62" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="D62" s="32"/>
-      <c r="E62" s="33"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="33"/>
-      <c r="H62" s="33"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="33"/>
-      <c r="K62" s="33"/>
-      <c r="L62" s="33"/>
-      <c r="M62" s="33"/>
-      <c r="N62" s="33"/>
-      <c r="O62" s="34"/>
-    </row>
-    <row r="63" spans="1:16" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="131"/>
-      <c r="B63" s="72" t="s">
-        <v>137</v>
-      </c>
-      <c r="C63" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D63" s="35" t="s">
-        <v>76</v>
-      </c>
-      <c r="E63" s="36"/>
-      <c r="F63" s="36"/>
-      <c r="G63" s="36"/>
-      <c r="H63" s="36"/>
-      <c r="I63" s="36"/>
-      <c r="J63" s="36"/>
-      <c r="K63" s="36"/>
-      <c r="L63" s="36"/>
-      <c r="M63" s="36"/>
-      <c r="N63" s="36"/>
-      <c r="O63" s="37"/>
-    </row>
-    <row r="64" spans="1:16" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="131"/>
-      <c r="B64" s="97" t="s">
-        <v>138</v>
-      </c>
-      <c r="C64" s="116" t="s">
-        <v>109</v>
-      </c>
-      <c r="D64" s="29" t="s">
-        <v>111</v>
-      </c>
-      <c r="E64" s="30"/>
-      <c r="F64" s="30"/>
-      <c r="G64" s="30"/>
-      <c r="H64" s="30"/>
-      <c r="I64" s="30"/>
-      <c r="J64" s="30"/>
-      <c r="K64" s="30"/>
-      <c r="L64" s="30"/>
-      <c r="M64" s="30"/>
-      <c r="N64" s="30"/>
-      <c r="O64" s="31"/>
-    </row>
-    <row r="65" spans="1:15" ht="95.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="131"/>
-      <c r="B65" s="96"/>
-      <c r="C65" s="5" t="s">
-        <v>110</v>
-      </c>
-      <c r="D65" s="32"/>
-      <c r="E65" s="33"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="33"/>
-      <c r="H65" s="33"/>
-      <c r="I65" s="33"/>
-      <c r="J65" s="33"/>
-      <c r="K65" s="33"/>
-      <c r="L65" s="33"/>
-      <c r="M65" s="33"/>
-      <c r="N65" s="33"/>
-      <c r="O65" s="34"/>
-    </row>
-    <row r="66" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="131"/>
-      <c r="B66" s="97" t="s">
-        <v>139</v>
-      </c>
-      <c r="C66" s="117" t="s">
-        <v>35</v>
-      </c>
-      <c r="D66" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E66" s="30"/>
-      <c r="F66" s="30"/>
-      <c r="G66" s="30"/>
-      <c r="H66" s="30"/>
-      <c r="I66" s="30"/>
-      <c r="J66" s="30"/>
-      <c r="K66" s="30"/>
-      <c r="L66" s="30"/>
-      <c r="M66" s="30"/>
-      <c r="N66" s="30"/>
-      <c r="O66" s="31"/>
-    </row>
-    <row r="67" spans="1:15" ht="83.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="131"/>
-      <c r="B67" s="96"/>
-      <c r="C67" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D67" s="32"/>
-      <c r="E67" s="33"/>
-      <c r="F67" s="33"/>
-      <c r="G67" s="33"/>
-      <c r="H67" s="33"/>
-      <c r="I67" s="33"/>
-      <c r="J67" s="33"/>
-      <c r="K67" s="33"/>
-      <c r="L67" s="33"/>
-      <c r="M67" s="33"/>
-      <c r="N67" s="33"/>
-      <c r="O67" s="34"/>
-    </row>
-    <row r="68" spans="1:15" ht="76.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="131"/>
-      <c r="B68" s="88" t="s">
-        <v>140</v>
-      </c>
-      <c r="C68" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D68" s="35" t="s">
-        <v>78</v>
-      </c>
-      <c r="E68" s="36"/>
-      <c r="F68" s="36"/>
-      <c r="G68" s="36"/>
-      <c r="H68" s="36"/>
-      <c r="I68" s="36"/>
-      <c r="J68" s="36"/>
-      <c r="K68" s="36"/>
-      <c r="L68" s="36"/>
-      <c r="M68" s="36"/>
-      <c r="N68" s="36"/>
-      <c r="O68" s="37"/>
-    </row>
-    <row r="69" spans="1:15" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="131"/>
-      <c r="B69" s="97" t="s">
-        <v>141</v>
-      </c>
-      <c r="C69" s="118" t="s">
-        <v>112</v>
-      </c>
-      <c r="D69" s="75" t="s">
-        <v>114</v>
-      </c>
-      <c r="E69" s="76"/>
       <c r="F69" s="76"/>
       <c r="G69" s="76"/>
       <c r="H69" s="76"/>
@@ -4925,16 +5103,17 @@
       <c r="L69" s="76"/>
       <c r="M69" s="76"/>
       <c r="N69" s="76"/>
-      <c r="O69" s="77"/>
-    </row>
-    <row r="70" spans="1:15" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="132"/>
-      <c r="B70" s="96"/>
-      <c r="C70" s="81" t="s">
-        <v>113</v>
-      </c>
-      <c r="D70" s="78"/>
-      <c r="E70" s="79"/>
+      <c r="O69" s="76"/>
+      <c r="P69" s="77"/>
+    </row>
+    <row r="70" spans="1:16" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="63"/>
+      <c r="B70" s="55"/>
+      <c r="C70" s="128"/>
+      <c r="D70" s="28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E70" s="78"/>
       <c r="F70" s="79"/>
       <c r="G70" s="79"/>
       <c r="H70" s="79"/>
@@ -4944,216 +5123,239 @@
       <c r="L70" s="79"/>
       <c r="M70" s="79"/>
       <c r="N70" s="79"/>
-      <c r="O70" s="80"/>
-    </row>
-    <row r="71" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="133" t="s">
+      <c r="O70" s="79"/>
+      <c r="P70" s="80"/>
+    </row>
+    <row r="71" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="122" t="s">
         <v>36</v>
       </c>
-      <c r="B71" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="C71" s="21" t="s">
+      <c r="B71" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="C71" s="140" t="s">
+        <v>155</v>
+      </c>
+      <c r="D71" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="D71" s="23" t="s">
+      <c r="E71" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
-      <c r="J71" s="24"/>
-      <c r="K71" s="24"/>
-      <c r="L71" s="24"/>
-      <c r="M71" s="24"/>
-      <c r="N71" s="24"/>
-      <c r="O71" s="25"/>
-    </row>
-    <row r="72" spans="1:15" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="134"/>
-      <c r="B72" s="91"/>
-      <c r="C72" s="6" t="s">
+      <c r="F71" s="73"/>
+      <c r="G71" s="73"/>
+      <c r="H71" s="73"/>
+      <c r="I71" s="73"/>
+      <c r="J71" s="73"/>
+      <c r="K71" s="73"/>
+      <c r="L71" s="73"/>
+      <c r="M71" s="73"/>
+      <c r="N71" s="73"/>
+      <c r="O71" s="73"/>
+      <c r="P71" s="74"/>
+    </row>
+    <row r="72" spans="1:16" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="123"/>
+      <c r="B72" s="138"/>
+      <c r="C72" s="141"/>
+      <c r="D72" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D72" s="26" t="s">
+      <c r="E72" s="115" t="s">
         <v>40</v>
       </c>
-      <c r="E72" s="27"/>
-      <c r="F72" s="27"/>
-      <c r="G72" s="27"/>
-      <c r="H72" s="27"/>
-      <c r="I72" s="27"/>
-      <c r="J72" s="27"/>
-      <c r="K72" s="27"/>
-      <c r="L72" s="27"/>
-      <c r="M72" s="27"/>
-      <c r="N72" s="27"/>
-      <c r="O72" s="28"/>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A73" s="134"/>
-      <c r="B73" s="91"/>
-      <c r="C73" s="119" t="s">
+      <c r="F72" s="116"/>
+      <c r="G72" s="116"/>
+      <c r="H72" s="116"/>
+      <c r="I72" s="116"/>
+      <c r="J72" s="116"/>
+      <c r="K72" s="116"/>
+      <c r="L72" s="116"/>
+      <c r="M72" s="116"/>
+      <c r="N72" s="116"/>
+      <c r="O72" s="116"/>
+      <c r="P72" s="117"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A73" s="123"/>
+      <c r="B73" s="138"/>
+      <c r="C73" s="141"/>
+      <c r="D73" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D73" s="29" t="s">
+      <c r="E73" s="75" t="s">
         <v>42</v>
       </c>
-      <c r="E73" s="30"/>
-      <c r="F73" s="30"/>
-      <c r="G73" s="30"/>
-      <c r="H73" s="30"/>
-      <c r="I73" s="30"/>
-      <c r="J73" s="30"/>
-      <c r="K73" s="30"/>
-      <c r="L73" s="30"/>
-      <c r="M73" s="30"/>
-      <c r="N73" s="30"/>
-      <c r="O73" s="31"/>
-    </row>
-    <row r="74" spans="1:15" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="134"/>
-      <c r="B74" s="91"/>
-      <c r="C74" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="D74" s="32"/>
-      <c r="E74" s="33"/>
-      <c r="F74" s="33"/>
-      <c r="G74" s="33"/>
-      <c r="H74" s="33"/>
-      <c r="I74" s="33"/>
-      <c r="J74" s="33"/>
-      <c r="K74" s="33"/>
-      <c r="L74" s="33"/>
-      <c r="M74" s="33"/>
-      <c r="N74" s="33"/>
-      <c r="O74" s="34"/>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="134"/>
-      <c r="B75" s="91"/>
-      <c r="C75" s="120" t="s">
+      <c r="F73" s="76"/>
+      <c r="G73" s="76"/>
+      <c r="H73" s="76"/>
+      <c r="I73" s="76"/>
+      <c r="J73" s="76"/>
+      <c r="K73" s="76"/>
+      <c r="L73" s="76"/>
+      <c r="M73" s="76"/>
+      <c r="N73" s="76"/>
+      <c r="O73" s="76"/>
+      <c r="P73" s="77"/>
+    </row>
+    <row r="74" spans="1:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="123"/>
+      <c r="B74" s="138"/>
+      <c r="C74" s="141"/>
+      <c r="D74" s="20" t="s">
+        <v>77</v>
+      </c>
+      <c r="E74" s="78"/>
+      <c r="F74" s="79"/>
+      <c r="G74" s="79"/>
+      <c r="H74" s="79"/>
+      <c r="I74" s="79"/>
+      <c r="J74" s="79"/>
+      <c r="K74" s="79"/>
+      <c r="L74" s="79"/>
+      <c r="M74" s="79"/>
+      <c r="N74" s="79"/>
+      <c r="O74" s="79"/>
+      <c r="P74" s="80"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A75" s="123"/>
+      <c r="B75" s="138"/>
+      <c r="C75" s="141"/>
+      <c r="D75" s="50" t="s">
         <v>43</v>
       </c>
-      <c r="D75" s="29" t="s">
+      <c r="E75" s="75" t="s">
         <v>44</v>
       </c>
-      <c r="E75" s="30"/>
-      <c r="F75" s="30"/>
-      <c r="G75" s="30"/>
-      <c r="H75" s="30"/>
-      <c r="I75" s="30"/>
-      <c r="J75" s="30"/>
-      <c r="K75" s="30"/>
-      <c r="L75" s="30"/>
-      <c r="M75" s="30"/>
-      <c r="N75" s="30"/>
-      <c r="O75" s="31"/>
-    </row>
-    <row r="76" spans="1:15" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="134"/>
-      <c r="B76" s="91"/>
-      <c r="C76" s="103" t="s">
-        <v>80</v>
-      </c>
-      <c r="D76" s="83"/>
-      <c r="E76" s="84"/>
-      <c r="F76" s="84"/>
-      <c r="G76" s="84"/>
-      <c r="H76" s="84"/>
-      <c r="I76" s="84"/>
-      <c r="J76" s="84"/>
-      <c r="K76" s="84"/>
-      <c r="L76" s="84"/>
-      <c r="M76" s="84"/>
-      <c r="N76" s="84"/>
-      <c r="O76" s="105"/>
-    </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A77" s="135"/>
-      <c r="B77" s="92"/>
-      <c r="C77" s="104"/>
-      <c r="D77" s="32"/>
-      <c r="E77" s="33"/>
-      <c r="F77" s="33"/>
-      <c r="G77" s="33"/>
-      <c r="H77" s="33"/>
-      <c r="I77" s="33"/>
-      <c r="J77" s="33"/>
-      <c r="K77" s="33"/>
-      <c r="L77" s="33"/>
-      <c r="M77" s="33"/>
-      <c r="N77" s="33"/>
-      <c r="O77" s="34"/>
+      <c r="F75" s="76"/>
+      <c r="G75" s="76"/>
+      <c r="H75" s="76"/>
+      <c r="I75" s="76"/>
+      <c r="J75" s="76"/>
+      <c r="K75" s="76"/>
+      <c r="L75" s="76"/>
+      <c r="M75" s="76"/>
+      <c r="N75" s="76"/>
+      <c r="O75" s="76"/>
+      <c r="P75" s="77"/>
+    </row>
+    <row r="76" spans="1:16" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="123"/>
+      <c r="B76" s="138"/>
+      <c r="C76" s="141"/>
+      <c r="D76" s="56" t="s">
+        <v>78</v>
+      </c>
+      <c r="E76" s="109"/>
+      <c r="F76" s="110"/>
+      <c r="G76" s="110"/>
+      <c r="H76" s="110"/>
+      <c r="I76" s="110"/>
+      <c r="J76" s="110"/>
+      <c r="K76" s="110"/>
+      <c r="L76" s="110"/>
+      <c r="M76" s="110"/>
+      <c r="N76" s="110"/>
+      <c r="O76" s="110"/>
+      <c r="P76" s="125"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A77" s="124"/>
+      <c r="B77" s="55"/>
+      <c r="C77" s="147"/>
+      <c r="D77" s="57"/>
+      <c r="E77" s="78"/>
+      <c r="F77" s="79"/>
+      <c r="G77" s="79"/>
+      <c r="H77" s="79"/>
+      <c r="I77" s="79"/>
+      <c r="J77" s="79"/>
+      <c r="K77" s="79"/>
+      <c r="L77" s="79"/>
+      <c r="M77" s="79"/>
+      <c r="N77" s="79"/>
+      <c r="O77" s="79"/>
+      <c r="P77" s="80"/>
     </row>
   </sheetData>
-  <mergeCells count="63">
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="B66:B67"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="C76:C77"/>
+  <mergeCells count="76">
+    <mergeCell ref="C33:C34"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="C37:C40"/>
+    <mergeCell ref="C41:C44"/>
+    <mergeCell ref="C47:C52"/>
+    <mergeCell ref="C22:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C27:C28"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E73:P74"/>
+    <mergeCell ref="A71:A77"/>
+    <mergeCell ref="B71:B77"/>
+    <mergeCell ref="E75:P77"/>
+    <mergeCell ref="E66:P67"/>
+    <mergeCell ref="E68:P68"/>
+    <mergeCell ref="C66:C70"/>
+    <mergeCell ref="C71:C77"/>
+    <mergeCell ref="E53:P54"/>
+    <mergeCell ref="E71:P71"/>
+    <mergeCell ref="E72:P72"/>
+    <mergeCell ref="E37:P38"/>
+    <mergeCell ref="E41:P42"/>
+    <mergeCell ref="E43:P44"/>
+    <mergeCell ref="E51:P52"/>
+    <mergeCell ref="E57:P58"/>
+    <mergeCell ref="E64:P65"/>
+    <mergeCell ref="E69:P70"/>
+    <mergeCell ref="E45:P45"/>
+    <mergeCell ref="E49:P49"/>
+    <mergeCell ref="E46:P46"/>
+    <mergeCell ref="E47:P48"/>
+    <mergeCell ref="E50:P50"/>
+    <mergeCell ref="E55:P55"/>
+    <mergeCell ref="E35:P36"/>
+    <mergeCell ref="E39:P40"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A18:R18"/>
+    <mergeCell ref="E19:P19"/>
+    <mergeCell ref="E20:P20"/>
+    <mergeCell ref="E21:P21"/>
+    <mergeCell ref="A20:A36"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="E29:P32"/>
     <mergeCell ref="A37:A44"/>
-    <mergeCell ref="A45:A58"/>
-    <mergeCell ref="A59:A70"/>
+    <mergeCell ref="E22:P23"/>
+    <mergeCell ref="E24:P24"/>
+    <mergeCell ref="E25:P26"/>
+    <mergeCell ref="E27:P28"/>
+    <mergeCell ref="E33:P34"/>
+    <mergeCell ref="E56:P56"/>
+    <mergeCell ref="E59:P59"/>
+    <mergeCell ref="E60:P60"/>
+    <mergeCell ref="E61:P62"/>
+    <mergeCell ref="E63:P63"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="B47:B48"/>
     <mergeCell ref="B27:B28"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="B33:B34"/>
     <mergeCell ref="B35:B36"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="D76:D77"/>
+    <mergeCell ref="A45:A58"/>
+    <mergeCell ref="A59:A70"/>
     <mergeCell ref="B51:B52"/>
     <mergeCell ref="B53:B54"/>
     <mergeCell ref="B57:B58"/>
-    <mergeCell ref="D43:O44"/>
-    <mergeCell ref="D51:O52"/>
-    <mergeCell ref="D57:O58"/>
-    <mergeCell ref="D64:O65"/>
-    <mergeCell ref="D69:O70"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="A18:Q18"/>
-    <mergeCell ref="D19:O19"/>
-    <mergeCell ref="D20:O20"/>
-    <mergeCell ref="D21:O21"/>
-    <mergeCell ref="A20:A36"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="D45:O45"/>
-    <mergeCell ref="D49:O49"/>
-    <mergeCell ref="D46:O46"/>
-    <mergeCell ref="D47:O48"/>
-    <mergeCell ref="D50:O50"/>
-    <mergeCell ref="D29:O32"/>
-    <mergeCell ref="D37:O38"/>
-    <mergeCell ref="D41:O42"/>
-    <mergeCell ref="D22:O23"/>
-    <mergeCell ref="D24:O24"/>
-    <mergeCell ref="D25:O26"/>
-    <mergeCell ref="D27:O28"/>
-    <mergeCell ref="D33:O34"/>
-    <mergeCell ref="D35:O36"/>
-    <mergeCell ref="D39:O40"/>
-    <mergeCell ref="D55:O55"/>
-    <mergeCell ref="D56:O56"/>
-    <mergeCell ref="D59:O59"/>
-    <mergeCell ref="D60:O60"/>
-    <mergeCell ref="D61:O62"/>
-    <mergeCell ref="D63:O63"/>
-    <mergeCell ref="D66:O67"/>
-    <mergeCell ref="D68:O68"/>
-    <mergeCell ref="D53:O54"/>
-    <mergeCell ref="D71:O71"/>
-    <mergeCell ref="D72:O72"/>
-    <mergeCell ref="D73:O74"/>
-    <mergeCell ref="A71:A77"/>
-    <mergeCell ref="B71:B77"/>
-    <mergeCell ref="D75:O77"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C53:C58"/>
+    <mergeCell ref="C61:C65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>